<commit_message>
adding testcases for registeration and cst main and account page
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Accounts TC.xlsx
+++ b/Testing/Test Cases/Accounts TC.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Internet-Banking-System\Internet-Banking-System\Testing\Test Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti\project managment\coding\Internet-Banking-System\Testing\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23004" windowHeight="8460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,257 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
+  <si>
+    <t>Project Name:</t>
+  </si>
+  <si>
+    <t>Internet Banking System</t>
+  </si>
+  <si>
+    <t>Test Designed by:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khadija Mostafa </t>
+  </si>
+  <si>
+    <t>Module Name:</t>
+  </si>
+  <si>
+    <t>Registeration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Designed date: </t>
+  </si>
+  <si>
+    <t>14/5/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precondition </t>
+  </si>
+  <si>
+    <t>SRS ID</t>
+  </si>
+  <si>
+    <t>Test Case ID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Expected Results</t>
+  </si>
+  <si>
+    <t>Actual Results</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Reviewed By</t>
+  </si>
+  <si>
+    <t>Review comments</t>
+  </si>
+  <si>
+    <t>1-Open google chrome 
+2- Navigate to URL "      "
+3- user logged in successfully .</t>
+  </si>
+  <si>
+    <t>1- click on the hyper link logout .</t>
+  </si>
+  <si>
+    <t>customer shall be redirected 
+to login page with empty fields.</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_PT_R035</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_ACC_R001</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_PT_R003</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_ACC_R002</t>
+  </si>
+  <si>
+    <t>1- click on show details button .</t>
+  </si>
+  <si>
+    <t>customer shall be redirected 
+tohis account page according to the account he choose to press his button.</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_PT_R034</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_ACC_R003</t>
+  </si>
+  <si>
+    <t>1- click on show  previous
+ transaction button .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer shall be redirected to his previous 
+transaction page according to the account he 
+choose to press his show previous transaction
+ button. </t>
+  </si>
+  <si>
+    <t>validate that customer can logout successfully 
+from his main/accounts page.</t>
+  </si>
+  <si>
+    <t>validate that customer can logout successfully 
+from his account page.</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_ACC_R004</t>
+  </si>
+  <si>
+    <t>1- click on show details button for
+ the first account .
+2- click on the hyper link logout .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate customer redirection to his previous
+ transaction page from the his account page. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate customer redirection to his previous transaction page from the his main/accounts page.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate customer redirection to  his account 
+pagefrom the his main/accounts page.   </t>
+  </si>
+  <si>
+    <t>1- click on show details button for
+ the first account .
+2- click on the hyper link previous transaction .</t>
+  </si>
+  <si>
+    <t>customer shall be redirected to his previous 
+transaction page of his current account.</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_PT_R008</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_ACC_R005</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_ACC_R006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate customer redirection to his transfer page from the his account page. </t>
+  </si>
+  <si>
+    <t>1- click on show details button for
+ the first account .
+2- click on the hyper link transfer .</t>
+  </si>
+  <si>
+    <t>customer shall be redirected to his transfer page of his current account.</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_PT_R007</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_PT_R004</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_ACC_R007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate that customer balance is displayed in 
+his account page </t>
+  </si>
+  <si>
+    <t>1- click on show details button for
+ the first account .
+2- check that the customer balance is displayed .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">account page shall display the Customer balance </t>
+  </si>
+  <si>
+    <t xml:space="preserve">account page shall display the account type 
+(current &amp; saving) </t>
+  </si>
+  <si>
+    <t>1- click on show details button for
+ the first account .
+2- check that the customer account 
+type is displayed .</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_ACC_R008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate that customer account type is displayed in his account page </t>
+  </si>
+  <si>
+    <t>functional</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>validate customer redirection to his main/accounts page from his account page .</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_ACC_R009</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_PT_R029</t>
+  </si>
+  <si>
+    <t>1- click on show details button for
+ the first account .
+2- click on the button accounts  .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer shall be redirected to his main/accounts page </t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_ACC_R010</t>
+  </si>
+  <si>
+    <t>validate customer redirection to his main/accounts page from his account page if he clicks back frombrowser bar .</t>
+  </si>
+  <si>
+    <t>1- click on show details button for
+ the first account .
+2- click on back  .</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_PT_R036</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,16 +281,82 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -50,12 +364,112 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,12 +750,393 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D18" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9:H18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" customWidth="1"/>
+    <col min="3" max="3" width="42.85546875" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" customWidth="1"/>
+    <col min="6" max="6" width="44" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:12" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="11"/>
+    </row>
+    <row r="6" spans="1:12" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="15"/>
+    </row>
+    <row r="7" spans="1:12" s="17" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:12" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" t="s">
+        <v>70</v>
+      </c>
+      <c r="I14" t="s">
+        <v>59</v>
+      </c>
+      <c r="J14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" t="s">
+        <v>70</v>
+      </c>
+      <c r="I15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I16" t="s">
+        <v>59</v>
+      </c>
+      <c r="J16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17" t="s">
+        <v>70</v>
+      </c>
+      <c r="I17" t="s">
+        <v>59</v>
+      </c>
+      <c r="J17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18" t="s">
+        <v>70</v>
+      </c>
+      <c r="I18" t="s">
+        <v>59</v>
+      </c>
+      <c r="J18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B5:K5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
upadte accounts module asper reviewer comments
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Accounts TC.xlsx
+++ b/Testing/Test Cases/Accounts TC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\Internet-Banking-System\Testing\Test Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti\project managment\testing\Internet-Banking-System\Testing\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -123,20 +123,6 @@
  transaction button .</t>
   </si>
   <si>
-    <t xml:space="preserve">customer shall be redirected to his previous 
-transaction page according to the account he 
-choose to press his show previous transaction
- button. </t>
-  </si>
-  <si>
-    <t>validate that customer can logout successfully 
-from his main/accounts page.</t>
-  </si>
-  <si>
-    <t>validate that customer can logout successfully 
-from his account page.</t>
-  </si>
-  <si>
     <t>BANK_SYS_TC_ACC_R004</t>
   </si>
   <si>
@@ -145,19 +131,11 @@
 2- click on the hyper link logout .</t>
   </si>
   <si>
-    <t xml:space="preserve">validate customer redirection to his previous
- transaction page from the his account page. </t>
-  </si>
-  <si>
     <t>1- click on show details button for
  the first account .
 2- click on the hyper link previous transaction .</t>
   </si>
   <si>
-    <t>customer shall be redirected to his previous 
-transaction page of his current account.</t>
-  </si>
-  <si>
     <t>BANK_SYS_SRS_PT_R008</t>
   </si>
   <si>
@@ -165,17 +143,11 @@
   </si>
   <si>
     <t>BANK_SYS_TC_ACC_R006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">validate customer redirection to his transfer page from the his account page. </t>
   </si>
   <si>
     <t>1- click on show details button for
  the first account .
 2- click on the hyper link transfer .</t>
-  </si>
-  <si>
-    <t>customer shall be redirected to his transfer page of his current account.</t>
   </si>
   <si>
     <t>BANK_SYS_SRS_PT_R007</t>
@@ -221,9 +193,6 @@
     <t>open</t>
   </si>
   <si>
-    <t>validate customer redirection to his main/accounts page from his account page .</t>
-  </si>
-  <si>
     <t>BANK_SYS_TC_ACC_R009</t>
   </si>
   <si>
@@ -255,10 +224,6 @@
     <t xml:space="preserve">Main/account page </t>
   </si>
   <si>
-    <t xml:space="preserve">validate customer redirection to  his account 
-page from the his main/accounts page.   </t>
-  </si>
-  <si>
     <t>validate customer redirection to his main/accounts page from his account page if he clicks back from browser bar .</t>
   </si>
   <si>
@@ -274,9 +239,6 @@
   <si>
     <t xml:space="preserve">in the description you
  should mention that redirection by pressing the button </t>
-  </si>
-  <si>
-    <t xml:space="preserve">validate customer redirection to his previous transaction page from  his main/accounts page.   </t>
   </si>
   <si>
     <t>the word "current account"
@@ -299,6 +261,44 @@
     <t>in the description you
  should mention that redirection by pressing the button .
 unclear expected result.</t>
+  </si>
+  <si>
+    <t>validate that customer can logout successfully 
+from his main/accounts page by clicking on logout hyper link.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate customer redirection to  his account 
+page from the his main/accounts page by clicking on accounts button.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate customer redirection to his previous transaction page from  his main/accounts page by clicking on previoustransaction button.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer shall be redirected to his previous 
+transaction page of the account he 
+choose to press his show "previous transaction"
+ button. </t>
+  </si>
+  <si>
+    <t>validate that customer can logout successfully 
+from his account page by clicking on logout hyper link.</t>
+  </si>
+  <si>
+    <t>customer shall be redirected to his previous 
+transaction page of the account from its page he clicked on the hyper link.</t>
+  </si>
+  <si>
+    <t>customer shall be redirected to his transfer page of the account from its page he clicked on the hyper link.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate customer redirection to his transfer page from the his account page by clicking on the transfer hyperlink. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate customer redirection to his previous
+ transaction page from the his account page by clicking on the previous accounts hyper link . </t>
+  </si>
+  <si>
+    <t>validate customer redirection to his main/accounts page from his account page by pressing the accounts button.</t>
   </si>
 </sst>
 </file>
@@ -784,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F6" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,7 +824,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>5</v>
@@ -908,10 +908,10 @@
         <v>19</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -919,7 +919,7 @@
         <v>24</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
@@ -928,19 +928,19 @@
         <v>22</v>
       </c>
       <c r="H9" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I9" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J9" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="K9" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="L9" s="18" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -951,28 +951,28 @@
         <v>26</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s">
         <v>27</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I10" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J10" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="K10" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="L10" s="18" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -983,28 +983,28 @@
         <v>29</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>30</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="H11" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I11" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J11" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="K11" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="L11" s="18" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -1012,214 +1012,214 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F12" s="18" t="s">
         <v>22</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I12" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J12" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="K12" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="L12" s="18" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="H13" t="s">
+        <v>57</v>
+      </c>
+      <c r="I13" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" t="s">
+        <v>49</v>
+      </c>
+      <c r="K13" t="s">
+        <v>60</v>
+      </c>
+      <c r="L13" s="18" t="s">
         <v>65</v>
-      </c>
-      <c r="I13" t="s">
-        <v>55</v>
-      </c>
-      <c r="J13" t="s">
-        <v>56</v>
-      </c>
-      <c r="K13" t="s">
-        <v>69</v>
-      </c>
-      <c r="L13" s="18" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="H14" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="K14" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="L14" s="18" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C15" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I15" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="J15" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="H15" t="s">
-        <v>65</v>
-      </c>
-      <c r="I15" t="s">
-        <v>55</v>
-      </c>
-      <c r="J15" t="s">
-        <v>56</v>
-      </c>
       <c r="K15" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" t="s">
-        <v>53</v>
-      </c>
       <c r="C16" s="18" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H16" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I16" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J16" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="K16" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C17" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="I17" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" t="s">
+        <v>49</v>
+      </c>
+      <c r="K17" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="H17" t="s">
-        <v>65</v>
-      </c>
-      <c r="I17" t="s">
-        <v>55</v>
-      </c>
-      <c r="J17" t="s">
-        <v>56</v>
-      </c>
-      <c r="K17" t="s">
-        <v>69</v>
-      </c>
       <c r="L17" s="18" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H18" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I18" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J18" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="K18" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update testcases as per reviewer comments
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Accounts TC.xlsx
+++ b/Testing/Test Cases/Accounts TC.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="90">
   <si>
     <t>Project Name:</t>
   </si>
@@ -299,6 +299,66 @@
   </si>
   <si>
     <t>validate customer redirection to his main/accounts page from his account page by pressing the accounts button.</t>
+  </si>
+  <si>
+    <t>created by</t>
+  </si>
+  <si>
+    <t>khadija mostafa</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_ACC_R011</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_ACC_R012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate that all elements are exist in the accounts /main page </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> main / accounts page contains 
+1- hyper link logout 
+2- all customer accounts with two buttons ( view previous transaction -show details)</t>
+  </si>
+  <si>
+    <t>validate that main / accounts page contains 
+1- hyper link logout 
+2- all customer accounts with two buttons ( view previous transaction -show details)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate that all elements are exist in the account page </t>
+  </si>
+  <si>
+    <t>validate that account page contains 
+1- hyper link logout 
+2- accounts button 
+3- customer account type 
+4- balance 
+5- transfer hyper link 
+previous transaction hyper link .</t>
+  </si>
+  <si>
+    <t>account page contains 
+1- hyper link logout 
+2- accounts button 
+3- customer account type 
+4- balance 
+5- transfer hyper link 
+previous transaction hyper link .</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_PT_R035
+BANK_SYS_SRS_PT_R04
+BANK_SYS_SRS_PT_R05
+BANK_SYS_SRS_PT_R06
+BANK_SYS_SRS_PT_R028</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_PT_R035
+BANK_SYS_SRS_PT_R001
+BANK_SYS_SRS_PT_R030
+BANK_SYS_SRS_PT_R026
+BANK_SYS_SRS_PT_R027</t>
   </si>
 </sst>
 </file>
@@ -782,10 +842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,13 +859,14 @@
     <col min="7" max="7" width="23.28515625" customWidth="1"/>
     <col min="8" max="8" width="15.140625" customWidth="1"/>
     <col min="9" max="9" width="24.85546875" customWidth="1"/>
-    <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="24.5703125" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" customWidth="1"/>
+    <col min="11" max="11" width="27.85546875" customWidth="1"/>
+    <col min="12" max="12" width="20" customWidth="1"/>
+    <col min="13" max="13" width="24.5703125" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -819,7 +880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
@@ -833,12 +894,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:13" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B5" s="20"/>
       <c r="C5" s="21"/>
       <c r="D5" s="21"/>
@@ -849,9 +910,10 @@
       <c r="I5" s="21"/>
       <c r="J5" s="21"/>
       <c r="K5" s="21"/>
-      <c r="L5" s="9"/>
-    </row>
-    <row r="6" spans="1:13" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="L5" s="21"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" spans="1:14" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -867,10 +929,11 @@
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
-      <c r="L6" s="13"/>
-    </row>
-    <row r="7" spans="1:13" s="15" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:13" s="17" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L6" s="12"/>
+      <c r="M6" s="13"/>
+    </row>
+    <row r="7" spans="1:14" s="15" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:14" s="17" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>8</v>
       </c>
@@ -902,16 +965,19 @@
         <v>17</v>
       </c>
       <c r="K8" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="L8" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="17" t="s">
+      <c r="M8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="17" t="s">
+      <c r="N8" s="17" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -937,13 +1003,16 @@
         <v>49</v>
       </c>
       <c r="K9" t="s">
+        <v>79</v>
+      </c>
+      <c r="L9" t="s">
         <v>60</v>
       </c>
-      <c r="L9" s="18" t="s">
+      <c r="M9" s="18" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -969,13 +1038,16 @@
         <v>49</v>
       </c>
       <c r="K10" t="s">
+        <v>79</v>
+      </c>
+      <c r="L10" t="s">
         <v>60</v>
       </c>
-      <c r="L10" s="18" t="s">
+      <c r="M10" s="18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>28</v>
       </c>
@@ -1001,13 +1073,16 @@
         <v>49</v>
       </c>
       <c r="K11" t="s">
+        <v>79</v>
+      </c>
+      <c r="L11" t="s">
         <v>60</v>
       </c>
-      <c r="L11" s="18" t="s">
+      <c r="M11" s="18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1033,13 +1108,16 @@
         <v>49</v>
       </c>
       <c r="K12" t="s">
+        <v>79</v>
+      </c>
+      <c r="L12" t="s">
         <v>60</v>
       </c>
-      <c r="L12" s="18" t="s">
+      <c r="M12" s="18" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1065,13 +1143,16 @@
         <v>49</v>
       </c>
       <c r="K13" t="s">
+        <v>79</v>
+      </c>
+      <c r="L13" t="s">
         <v>60</v>
       </c>
-      <c r="L13" s="18" t="s">
+      <c r="M13" s="18" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1097,13 +1178,16 @@
         <v>49</v>
       </c>
       <c r="K14" t="s">
+        <v>79</v>
+      </c>
+      <c r="L14" t="s">
         <v>60</v>
       </c>
-      <c r="L14" s="18" t="s">
+      <c r="M14" s="18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1129,10 +1213,13 @@
         <v>49</v>
       </c>
       <c r="K15" t="s">
+        <v>79</v>
+      </c>
+      <c r="L15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1158,10 +1245,13 @@
         <v>49</v>
       </c>
       <c r="K16" t="s">
+        <v>79</v>
+      </c>
+      <c r="L16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -1187,13 +1277,16 @@
         <v>49</v>
       </c>
       <c r="K17" t="s">
+        <v>79</v>
+      </c>
+      <c r="L17" t="s">
         <v>60</v>
       </c>
-      <c r="L17" s="18" t="s">
+      <c r="M17" s="18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1219,12 +1312,73 @@
         <v>49</v>
       </c>
       <c r="K18" t="s">
+        <v>79</v>
+      </c>
+      <c r="L18" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="H19" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" t="s">
+        <v>48</v>
+      </c>
+      <c r="J19" t="s">
+        <v>49</v>
+      </c>
+      <c r="K19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="H20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J20" t="s">
+        <v>49</v>
+      </c>
+      <c r="K20" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="B5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>